<commit_message>
Add release products, license and readme to repository
</commit_message>
<xml_diff>
--- a/Release_Products/BOM_Mouser_Manual_Assy.xlsx
+++ b/Release_Products/BOM_Mouser_Manual_Assy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Driver_Modulation\Release_Products\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ECA93FD-6BA3-4D98-B918-92E41896A020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808528FD-A567-47D3-BA95-283A1EA05F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{57C99D80-BCAD-4B02-A02F-789964E46F5D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="124">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -119,15 +119,15 @@
     <t>AUD</t>
   </si>
   <si>
+    <t>68000-406HLF</t>
+  </si>
+  <si>
     <t>22-28-4020</t>
   </si>
   <si>
     <t>22-28-4080</t>
   </si>
   <si>
-    <t>68000-406HLF</t>
-  </si>
-  <si>
     <t>10129378-903001BLF</t>
   </si>
   <si>
@@ -164,15 +164,15 @@
     <t>U.FL-R-SMT-1(01)</t>
   </si>
   <si>
+    <t>CONN HEADER 6POS .100 STR TIN</t>
+  </si>
+  <si>
     <t>KK 254 Breakaway Header, Vertical, 2 Circuits, Tin (Sn) Plating, Mating Pin Length 6.09mm 2 POS</t>
   </si>
   <si>
     <t>Conn Unshrouded Header HDR 8 POS 2.54mm Solder ST Thru-Hole Bag</t>
   </si>
   <si>
-    <t>CONN HEADER 6POS .100 STR TIN</t>
-  </si>
-  <si>
     <t>Conn Unshrouded Header HDR 3 POS 2.54mm Solder ST Thru-Hole Poly Bag</t>
   </si>
   <si>
@@ -209,13 +209,16 @@
     <t>Rf Connectors / Coaxial Connectors SMT Ml Rec Au 50 Ohm W/anti Sldr Wicking UFL</t>
   </si>
   <si>
+    <t>J13</t>
+  </si>
+  <si>
     <t>J2, J9, J14</t>
   </si>
   <si>
     <t>J11, J12</t>
   </si>
   <si>
-    <t>J5, J10, J13</t>
+    <t>J5, J10</t>
   </si>
   <si>
     <t>J1, J4, J6</t>
@@ -254,6 +257,9 @@
     <t>E6, E7, E9, E10, E11</t>
   </si>
   <si>
+    <t>CMP-00021-3</t>
+  </si>
+  <si>
     <t>CMP-00157-5</t>
   </si>
   <si>
@@ -314,6 +320,9 @@
     <t>C7835</t>
   </si>
   <si>
+    <t>Amphenol Communications Solutions</t>
+  </si>
+  <si>
     <t>AMPHENOL ICC (FCI)</t>
   </si>
   <si>
@@ -329,7 +338,7 @@
     <t>Optek</t>
   </si>
   <si>
-    <t>SHOU HAN</t>
+    <t>C&amp;K Components</t>
   </si>
   <si>
     <t>Osram</t>
@@ -356,9 +365,6 @@
     <t>OPV314</t>
   </si>
   <si>
-    <t>MSK12C02-HB</t>
-  </si>
-  <si>
     <t>HPC5040NF-470M</t>
   </si>
   <si>
@@ -380,7 +386,7 @@
     <t>863-NCP114ASN270T1G</t>
   </si>
   <si>
-    <t>C431541</t>
+    <t>C221841</t>
   </si>
   <si>
     <t>720-SFH203P</t>
@@ -1324,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6FAA5-F42B-4942-B878-D6F4C02FDE8B}">
-  <dimension ref="B1:P36"/>
+  <dimension ref="B1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,28 +1533,28 @@
         <v>20</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I13" s="35" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="K13" s="35" t="s">
         <v>5</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M13" s="35" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="N13" s="35" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="O13" s="36" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="P13" s="37"/>
     </row>
@@ -1564,19 +1570,23 @@
         <v>57</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H14" s="20"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="I14" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
       <c r="M14" s="15"/>
       <c r="N14" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O14" s="22"/>
       <c r="P14" s="5"/>
@@ -1593,10 +1603,10 @@
         <v>58</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="14"/>
@@ -1605,12 +1615,12 @@
       <c r="L15" s="14"/>
       <c r="M15" s="15"/>
       <c r="N15" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O15" s="22"/>
       <c r="P15" s="5"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="13" t="s">
         <v>29</v>
@@ -1622,10 +1632,10 @@
         <v>59</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="14"/>
@@ -1634,531 +1644,555 @@
       <c r="L16" s="14"/>
       <c r="M16" s="15"/>
       <c r="N16" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O16" s="22"/>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>60</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H17" s="20"/>
-      <c r="I17" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
       <c r="M17" s="15"/>
       <c r="N17" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O17" s="22"/>
       <c r="P17" s="5"/>
     </row>
-    <row r="18" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B18" s="21"/>
       <c r="C18" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>61</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="14" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K18" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M18" s="15">
-        <v>0.4</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
       <c r="N18" s="14">
-        <v>1</v>
-      </c>
-      <c r="O18" s="22">
-        <v>0.8</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="O18" s="22"/>
       <c r="P18" s="5"/>
     </row>
     <row r="19" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B19" s="21"/>
       <c r="C19" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H19" s="20"/>
       <c r="I19" s="14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="M19" s="15">
         <v>0.4</v>
       </c>
       <c r="N19" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O19" s="22">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="P19" s="5"/>
     </row>
-    <row r="20" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B20" s="21"/>
       <c r="C20" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>63</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H20" s="20"/>
       <c r="I20" s="14" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="M20" s="15">
-        <v>0.35787000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="N20" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O20" s="22">
-        <v>1.79</v>
+        <v>1.6</v>
       </c>
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B21" s="21"/>
       <c r="C21" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>64</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M21" s="15">
-        <v>0.26255000000000001</v>
+        <v>0.35861999999999999</v>
       </c>
       <c r="N21" s="14">
         <v>1</v>
       </c>
       <c r="O21" s="22">
-        <v>0.52510000000000001</v>
+        <v>1.79</v>
       </c>
       <c r="P21" s="5"/>
     </row>
     <row r="22" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B22" s="21"/>
       <c r="C22" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>65</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="M22" s="15">
+        <v>0.26255000000000001</v>
+      </c>
       <c r="N22" s="14">
         <v>1</v>
       </c>
-      <c r="O22" s="22"/>
+      <c r="O22" s="22">
+        <v>0.52510000000000001</v>
+      </c>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
       <c r="C23" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>66</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H23" s="20"/>
       <c r="I23" s="14" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="K23" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="M23" s="15">
-        <v>8.2780000000000006E-2</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="15"/>
       <c r="N23" s="14">
         <v>1</v>
       </c>
-      <c r="O23" s="22">
-        <v>0.82779999999999998</v>
-      </c>
+      <c r="O23" s="22"/>
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
       <c r="C24" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>67</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H24" s="20"/>
       <c r="I24" s="14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M24" s="15">
-        <v>1.48</v>
+        <v>0.2069</v>
       </c>
       <c r="N24" s="14">
         <v>1</v>
       </c>
       <c r="O24" s="22">
-        <v>2.97</v>
+        <v>0.41381000000000001</v>
       </c>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
       <c r="C25" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>68</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L25" s="14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M25" s="15">
-        <v>0.81852999999999998</v>
+        <v>1.48</v>
       </c>
       <c r="N25" s="14">
         <v>1</v>
       </c>
       <c r="O25" s="22">
-        <v>1.64</v>
+        <v>2.97</v>
       </c>
       <c r="P25" s="5"/>
     </row>
     <row r="26" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B26" s="21"/>
       <c r="C26" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>69</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>91</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H26" s="20"/>
       <c r="I26" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L26" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="M26" s="15">
-        <v>0.44788</v>
+        <v>0.81852999999999998</v>
       </c>
       <c r="N26" s="14">
         <v>1</v>
       </c>
       <c r="O26" s="22">
-        <v>0.89575000000000005</v>
+        <v>1.64</v>
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B27" s="21"/>
       <c r="C27" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>70</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="H27" s="20"/>
+        <v>90</v>
+      </c>
+      <c r="H27" s="20" t="s">
+        <v>93</v>
+      </c>
       <c r="I27" s="14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J27" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="15"/>
+        <v>39</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M27" s="15">
+        <v>0.44788</v>
+      </c>
       <c r="N27" s="14">
         <v>1</v>
       </c>
-      <c r="O27" s="22"/>
+      <c r="O27" s="22">
+        <v>0.89575000000000005</v>
+      </c>
       <c r="P27" s="5"/>
     </row>
-    <row r="28" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B28" s="21"/>
       <c r="C28" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>71</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H28" s="20"/>
       <c r="I28" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="K28" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="L28" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="M28" s="15">
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="14">
+        <v>1</v>
+      </c>
+      <c r="O28" s="22"/>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="2:16" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B29" s="21"/>
+      <c r="C29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="20"/>
+      <c r="I29" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="M29" s="15">
         <v>5.8300000000000001E-3</v>
       </c>
-      <c r="N28" s="14">
+      <c r="N29" s="14">
         <v>5</v>
       </c>
-      <c r="O28" s="22">
+      <c r="O29" s="22">
         <v>5.8340000000000003E-2</v>
       </c>
-      <c r="P28" s="5"/>
-    </row>
-    <row r="29" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24">
-        <f>SUM(N14:N28)</f>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="23"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24">
+        <f>SUM(N14:N29)</f>
         <v>27</v>
       </c>
-      <c r="O29" s="25">
-        <f>SUM(O14:O28)</f>
-        <v>11.10699</v>
-      </c>
-      <c r="P29" s="5"/>
-    </row>
-    <row r="30" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="27" t="s">
+      <c r="O30" s="25">
+        <f>SUM(O14:O29)</f>
+        <v>10.693</v>
+      </c>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O31" s="4"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="26" t="s">
+      <c r="C32" s="9"/>
+      <c r="D32" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="9"/>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-      <c r="C32" s="10"/>
-      <c r="O32" s="10"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="9"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
@@ -2175,21 +2209,26 @@
       <c r="C35" s="10"/>
       <c r="O35" s="10"/>
     </row>
-    <row r="36" spans="2:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="12"/>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="10"/>
+      <c r="O36" s="10"/>
+    </row>
+    <row r="37" spans="2:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>